<commit_message>
rewrote lookup logic to be more robust and works with wildcards now. Still need to clean up code and do more testing
</commit_message>
<xml_diff>
--- a/tests/testdata/test_rating_tables_simple.xlsx
+++ b/tests/testdata/test_rating_tables_simple.xlsx
@@ -5,18 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="rating_table_numeric" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="rating_table_range" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="rating_table_boolean" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="rating_table_string" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="rating_table_numeric_wildcard" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="rating_table_range_wildcard" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="rating_table_boolean_wildcard" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="rating_table_string_wildcard" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="rating_table_combo" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="rating_table_numeric_wildcard" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="rating_table_range" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="rating_table_boolean" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="rating_table_string" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="rating_table_combo" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="12">
   <si>
     <t xml:space="preserve">_age</t>
   </si>
   <si>
     <t xml:space="preserve">factor_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
   </si>
   <si>
     <t xml:space="preserve">_age_left</t>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t xml:space="preserve">_safe_driving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">_credit_tier</t>
@@ -67,18 +61,6 @@
   </si>
   <si>
     <t xml:space="preserve">E1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X1</t>
   </si>
 </sst>
 </file>
@@ -186,11 +168,11 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -280,22 +262,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -304,76 +283,71 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="C2" s="1" t="n">
         <v>1.8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="n">
         <v>1.9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="C5" s="1" t="n">
         <v>2.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="C6" s="1" t="n">
         <v>2.2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="C7" s="1" t="n">
         <v>2.3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="C8" s="1" t="n">
         <v>2.4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -392,36 +366,111 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="1" t="n">
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1.8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
+      <c r="A3" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>1.5</v>
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -440,60 +489,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y24" activeCellId="0" sqref="Y24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
+      <c r="A2" s="2" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
+      <c r="A3" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>1.8</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -512,92 +538,68 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>18</v>
+      <c r="A2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>1.8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1" t="n">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>23</v>
-      </c>
       <c r="B7" s="1" t="n">
-        <v>2.3</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -616,22 +618,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -640,260 +648,13 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>2.3</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>2.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E40" activeCellId="0" sqref="E40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="C2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E48"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B45" activeCellId="0" sqref="B45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -906,11 +667,11 @@
       <c r="B3" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
+      <c r="C3" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="n">
         <f aca="false">E2+0.1</f>
@@ -924,11 +685,11 @@
       <c r="B4" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
+      <c r="C4" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="n">
         <f aca="false">E3+0.1</f>
@@ -942,11 +703,11 @@
       <c r="B5" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
+      <c r="C5" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="n">
         <f aca="false">E4+0.1</f>
@@ -960,11 +721,11 @@
       <c r="B6" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
+      <c r="C6" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1" t="n">
         <f aca="false">E5+0.1</f>
@@ -978,11 +739,11 @@
       <c r="B7" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
+      <c r="C7" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1" t="n">
         <f aca="false">E6+0.1</f>
@@ -996,11 +757,11 @@
       <c r="B8" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
+      <c r="C8" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1" t="n">
         <f aca="false">E7+0.1</f>
@@ -1014,11 +775,11 @@
       <c r="B9" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
+      <c r="C9" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="1" t="n">
         <f aca="false">E8+0.1</f>
@@ -1032,11 +793,11 @@
       <c r="B10" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>15</v>
+      <c r="C10" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1" t="n">
         <f aca="false">E9+0.1</f>
@@ -1050,11 +811,11 @@
       <c r="B11" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
+      <c r="C11" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1" t="n">
         <f aca="false">E10+0.1</f>
@@ -1068,11 +829,11 @@
       <c r="B12" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
+      <c r="C12" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1" t="n">
         <f aca="false">E11+0.1</f>
@@ -1086,11 +847,11 @@
       <c r="B13" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>15</v>
+      <c r="C13" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1" t="n">
         <f aca="false">E12+0.1</f>
@@ -1104,11 +865,11 @@
       <c r="B14" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>15</v>
+      <c r="C14" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" s="1" t="n">
         <f aca="false">E13+0.1</f>
@@ -1122,11 +883,11 @@
       <c r="B15" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>15</v>
+      <c r="C15" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="1" t="n">
         <f aca="false">E14+0.1</f>
@@ -1140,11 +901,11 @@
       <c r="B16" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>14</v>
+      <c r="C16" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="1" t="n">
         <f aca="false">E15+0.1</f>
@@ -1158,11 +919,11 @@
       <c r="B17" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>14</v>
+      <c r="C17" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="1" t="n">
         <f aca="false">E16+0.1</f>
@@ -1176,11 +937,11 @@
       <c r="B18" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>14</v>
+      <c r="C18" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="1" t="n">
         <f aca="false">E17+0.1</f>
@@ -1194,11 +955,11 @@
       <c r="B19" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>14</v>
+      <c r="C19" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" s="1" t="n">
         <f aca="false">E18+0.1</f>
@@ -1212,11 +973,11 @@
       <c r="B20" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>14</v>
+      <c r="C20" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20" s="1" t="n">
         <f aca="false">E19+0.1</f>
@@ -1230,11 +991,11 @@
       <c r="B21" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>14</v>
+      <c r="C21" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E21" s="1" t="n">
         <f aca="false">E20+0.1</f>
@@ -1248,11 +1009,11 @@
       <c r="B22" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>14</v>
+      <c r="C22" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E22" s="1" t="n">
         <f aca="false">E21+0.1</f>
@@ -1266,11 +1027,11 @@
       <c r="B23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>15</v>
+      <c r="C23" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E23" s="1" t="n">
         <f aca="false">E22+0.1</f>
@@ -1284,11 +1045,11 @@
       <c r="B24" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>15</v>
+      <c r="C24" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24" s="1" t="n">
         <f aca="false">E23+0.1</f>
@@ -1302,11 +1063,11 @@
       <c r="B25" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>15</v>
+      <c r="C25" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25" s="1" t="n">
         <f aca="false">E24+0.1</f>
@@ -1320,11 +1081,11 @@
       <c r="B26" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>15</v>
+      <c r="C26" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26" s="1" t="n">
         <f aca="false">E25+0.1</f>
@@ -1338,11 +1099,11 @@
       <c r="B27" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>15</v>
+      <c r="C27" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27" s="1" t="n">
         <f aca="false">E26+0.1</f>
@@ -1356,11 +1117,11 @@
       <c r="B28" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>15</v>
+      <c r="C28" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" s="1" t="n">
         <f aca="false">E27+0.1</f>
@@ -1374,11 +1135,11 @@
       <c r="B29" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>15</v>
+      <c r="C29" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E29" s="1" t="n">
         <f aca="false">E28+0.1</f>
@@ -1392,11 +1153,11 @@
       <c r="B30" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>14</v>
+      <c r="C30" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E30" s="1" t="n">
         <f aca="false">E29+0.1</f>
@@ -1410,11 +1171,11 @@
       <c r="B31" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>14</v>
+      <c r="C31" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E31" s="1" t="n">
         <f aca="false">E30+0.1</f>
@@ -1428,11 +1189,11 @@
       <c r="B32" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>14</v>
+      <c r="C32" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E32" s="1" t="n">
         <f aca="false">E31+0.1</f>
@@ -1446,11 +1207,11 @@
       <c r="B33" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>14</v>
+      <c r="C33" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33" s="1" t="n">
         <f aca="false">E32+0.1</f>
@@ -1464,11 +1225,11 @@
       <c r="B34" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>14</v>
+      <c r="C34" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E34" s="1" t="n">
         <f aca="false">E33+0.1</f>
@@ -1482,11 +1243,11 @@
       <c r="B35" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>14</v>
+      <c r="C35" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E35" s="1" t="n">
         <f aca="false">E34+0.1</f>
@@ -1500,11 +1261,11 @@
       <c r="B36" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>14</v>
+      <c r="C36" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36" s="1" t="n">
         <f aca="false">E35+0.1</f>
@@ -1518,11 +1279,11 @@
       <c r="B37" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>15</v>
+      <c r="C37" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E37" s="1" t="n">
         <f aca="false">E36+0.1</f>
@@ -1536,11 +1297,11 @@
       <c r="B38" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>15</v>
+      <c r="C38" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E38" s="1" t="n">
         <f aca="false">E37+0.1</f>
@@ -1554,11 +1315,11 @@
       <c r="B39" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>15</v>
+      <c r="C39" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E39" s="1" t="n">
         <f aca="false">E38+0.1</f>
@@ -1572,11 +1333,11 @@
       <c r="B40" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>15</v>
+      <c r="C40" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">E39+0.1</f>
@@ -1590,11 +1351,11 @@
       <c r="B41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>15</v>
+      <c r="C41" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E41" s="1" t="n">
         <f aca="false">E40+0.1</f>
@@ -1608,11 +1369,11 @@
       <c r="B42" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>15</v>
+      <c r="C42" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E42" s="1" t="n">
         <f aca="false">E41+0.1</f>
@@ -1626,11 +1387,11 @@
       <c r="B43" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>15</v>
+      <c r="C43" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E43" s="1" t="n">
         <f aca="false">E42+0.1</f>
@@ -1638,17 +1399,17 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B44" s="1" t="n">
-        <v>22</v>
+      <c r="A44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E44" s="1" t="n">
         <v>100</v>

</xml_diff>

<commit_message>
- Finished testing lookup functions - cleaned up code
</commit_message>
<xml_diff>
--- a/tests/testdata/test_rating_tables_simple.xlsx
+++ b/tests/testdata/test_rating_tables_simple.xlsx
@@ -5,15 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="rating_table_numeric" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="rating_table_numeric_wildcard" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="rating_table_range" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="rating_table_boolean" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="rating_table_string" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="rating_table_combo" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="rating_table_range" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="rating_table_boolean" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="rating_table_string" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="rating_table_combo" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="13">
   <si>
     <t xml:space="preserve">_age</t>
   </si>
   <si>
-    <t xml:space="preserve">factor_</t>
+    <t xml:space="preserve">factor0_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor1_</t>
   </si>
   <si>
     <t xml:space="preserve">*</t>
@@ -67,9 +69,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -136,7 +139,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -145,7 +148,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -166,10 +173,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -181,6 +188,9 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -189,6 +199,10 @@
       <c r="B2" s="1" t="n">
         <v>1.8</v>
       </c>
+      <c r="C2" s="2" t="n">
+        <f aca="false">B2+1</f>
+        <v>2.8</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -197,6 +211,10 @@
       <c r="B3" s="1" t="n">
         <v>1.9</v>
       </c>
+      <c r="C3" s="2" t="n">
+        <f aca="false">B3+1</f>
+        <v>2.9</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -205,6 +223,10 @@
       <c r="B4" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="C4" s="2" t="n">
+        <f aca="false">B4+1</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -213,6 +235,10 @@
       <c r="B5" s="1" t="n">
         <v>2.1</v>
       </c>
+      <c r="C5" s="2" t="n">
+        <f aca="false">B5+1</f>
+        <v>3.1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -221,6 +247,10 @@
       <c r="B6" s="1" t="n">
         <v>2.2</v>
       </c>
+      <c r="C6" s="2" t="n">
+        <f aca="false">B6+1</f>
+        <v>3.2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -229,6 +259,10 @@
       <c r="B7" s="1" t="n">
         <v>2.3</v>
       </c>
+      <c r="C7" s="2" t="n">
+        <f aca="false">B7+1</f>
+        <v>3.3</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -237,6 +271,10 @@
       <c r="B8" s="1" t="n">
         <v>2.4</v>
       </c>
+      <c r="C8" s="2" t="n">
+        <f aca="false">B8+1</f>
+        <v>3.4</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -245,11 +283,27 @@
       <c r="B9" s="1" t="n">
         <v>2.5</v>
       </c>
+      <c r="C9" s="2" t="n">
+        <f aca="false">B9+1</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <f aca="false">B10+1</f>
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -262,20 +316,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -283,72 +343,123 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>1.8</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <f aca="false">C2+1</f>
+        <v>2.8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>1.9</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <f aca="false">C3+1</f>
+        <v>2.9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <f aca="false">C4+1</f>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>2.1</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <f aca="false">C5+1</f>
+        <v>3.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="n">
         <v>2.2</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <f aca="false">C6+1</f>
+        <v>3.2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="n">
         <v>2.3</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <f aca="false">C7+1</f>
+        <v>3.3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B8" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="n">
         <v>2.4</v>
       </c>
+      <c r="D8" s="2" t="n">
+        <f aca="false">C8+1</f>
+        <v>3.4</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>2.5</v>
+      <c r="A9" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <f aca="false">C9+1</f>
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>3</v>
-      </c>
+      <c r="D10" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -366,112 +477,70 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <f aca="false">B2+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <f aca="false">B3+1</f>
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>1.9</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>2</v>
-      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>2.1</v>
-      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>2.2</v>
-      </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>2.3</v>
-      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>2.4</v>
-      </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>3</v>
-      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -489,38 +558,105 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y24" activeCellId="0" sqref="Y24"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="C2" s="2" t="n">
+        <f aca="false">B2+1</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <f aca="false">B3+1</f>
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <f aca="false">B4+1</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <f aca="false">B5+1</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <f aca="false">B6+1</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>3</v>
-      </c>
+      <c r="C7" s="2" t="n">
+        <f aca="false">B7+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -538,109 +674,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -650,14 +709,18 @@
       <c r="B2" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="b">
+      <c r="C2" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <f aca="false">E2+1</f>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -667,16 +730,20 @@
       <c r="B3" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C3" s="2" t="b">
+      <c r="C3" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="n">
         <f aca="false">E2+0.1</f>
         <v>1.1</v>
       </c>
+      <c r="F3" s="2" t="n">
+        <f aca="false">E3+1</f>
+        <v>2.1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -685,16 +752,20 @@
       <c r="B4" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C4" s="2" t="b">
+      <c r="C4" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="n">
         <f aca="false">E3+0.1</f>
         <v>1.2</v>
       </c>
+      <c r="F4" s="2" t="n">
+        <f aca="false">E4+1</f>
+        <v>2.2</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -703,16 +774,20 @@
       <c r="B5" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C5" s="2" t="b">
+      <c r="C5" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="n">
         <f aca="false">E4+0.1</f>
         <v>1.3</v>
       </c>
+      <c r="F5" s="2" t="n">
+        <f aca="false">E5+1</f>
+        <v>2.3</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -721,16 +796,20 @@
       <c r="B6" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C6" s="2" t="b">
+      <c r="C6" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="n">
         <f aca="false">E5+0.1</f>
         <v>1.4</v>
       </c>
+      <c r="F6" s="2" t="n">
+        <f aca="false">E6+1</f>
+        <v>2.4</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -739,16 +818,20 @@
       <c r="B7" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C7" s="2" t="b">
+      <c r="C7" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="n">
         <f aca="false">E6+0.1</f>
         <v>1.5</v>
       </c>
+      <c r="F7" s="2" t="n">
+        <f aca="false">E7+1</f>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -757,16 +840,20 @@
       <c r="B8" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C8" s="2" t="b">
+      <c r="C8" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="n">
         <f aca="false">E7+0.1</f>
         <v>1.6</v>
       </c>
+      <c r="F8" s="2" t="n">
+        <f aca="false">E8+1</f>
+        <v>2.6</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -775,16 +862,20 @@
       <c r="B9" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="b">
+      <c r="C9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="n">
         <f aca="false">E8+0.1</f>
         <v>1.7</v>
       </c>
+      <c r="F9" s="2" t="n">
+        <f aca="false">E9+1</f>
+        <v>2.7</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -793,16 +884,20 @@
       <c r="B10" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C10" s="2" t="b">
+      <c r="C10" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="n">
         <f aca="false">E9+0.1</f>
         <v>1.8</v>
       </c>
+      <c r="F10" s="2" t="n">
+        <f aca="false">E10+1</f>
+        <v>2.8</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -811,16 +906,20 @@
       <c r="B11" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C11" s="2" t="b">
+      <c r="C11" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1" t="n">
         <f aca="false">E10+0.1</f>
         <v>1.9</v>
       </c>
+      <c r="F11" s="2" t="n">
+        <f aca="false">E11+1</f>
+        <v>2.9</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -829,16 +928,20 @@
       <c r="B12" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C12" s="2" t="b">
+      <c r="C12" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E12" s="1" t="n">
         <f aca="false">E11+0.1</f>
         <v>2</v>
       </c>
+      <c r="F12" s="2" t="n">
+        <f aca="false">E12+1</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -847,16 +950,20 @@
       <c r="B13" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C13" s="2" t="b">
+      <c r="C13" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" s="1" t="n">
         <f aca="false">E12+0.1</f>
         <v>2.1</v>
       </c>
+      <c r="F13" s="2" t="n">
+        <f aca="false">E13+1</f>
+        <v>3.1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -865,16 +972,20 @@
       <c r="B14" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C14" s="2" t="b">
+      <c r="C14" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E14" s="1" t="n">
         <f aca="false">E13+0.1</f>
         <v>2.2</v>
       </c>
+      <c r="F14" s="2" t="n">
+        <f aca="false">E14+1</f>
+        <v>3.2</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -883,16 +994,20 @@
       <c r="B15" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C15" s="2" t="b">
+      <c r="C15" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1" t="n">
         <f aca="false">E14+0.1</f>
         <v>2.3</v>
       </c>
+      <c r="F15" s="2" t="n">
+        <f aca="false">E15+1</f>
+        <v>3.3</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -901,16 +1016,20 @@
       <c r="B16" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C16" s="2" t="b">
+      <c r="C16" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E16" s="1" t="n">
         <f aca="false">E15+0.1</f>
         <v>2.4</v>
       </c>
+      <c r="F16" s="2" t="n">
+        <f aca="false">E16+1</f>
+        <v>3.4</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -919,16 +1038,20 @@
       <c r="B17" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C17" s="2" t="b">
+      <c r="C17" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E17" s="1" t="n">
         <f aca="false">E16+0.1</f>
         <v>2.5</v>
       </c>
+      <c r="F17" s="2" t="n">
+        <f aca="false">E17+1</f>
+        <v>3.5</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -937,16 +1060,20 @@
       <c r="B18" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C18" s="2" t="b">
+      <c r="C18" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E18" s="1" t="n">
         <f aca="false">E17+0.1</f>
         <v>2.6</v>
       </c>
+      <c r="F18" s="2" t="n">
+        <f aca="false">E18+1</f>
+        <v>3.6</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -955,16 +1082,20 @@
       <c r="B19" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C19" s="2" t="b">
+      <c r="C19" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E19" s="1" t="n">
         <f aca="false">E18+0.1</f>
         <v>2.7</v>
       </c>
+      <c r="F19" s="2" t="n">
+        <f aca="false">E19+1</f>
+        <v>3.7</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -973,16 +1104,20 @@
       <c r="B20" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C20" s="2" t="b">
+      <c r="C20" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E20" s="1" t="n">
         <f aca="false">E19+0.1</f>
         <v>2.8</v>
       </c>
+      <c r="F20" s="2" t="n">
+        <f aca="false">E20+1</f>
+        <v>3.8</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -991,16 +1126,20 @@
       <c r="B21" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C21" s="2" t="b">
+      <c r="C21" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E21" s="1" t="n">
         <f aca="false">E20+0.1</f>
         <v>2.9</v>
       </c>
+      <c r="F21" s="2" t="n">
+        <f aca="false">E21+1</f>
+        <v>3.9</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -1009,15 +1148,19 @@
       <c r="B22" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C22" s="2" t="b">
+      <c r="C22" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E22" s="1" t="n">
         <f aca="false">E21+0.1</f>
         <v>3</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <f aca="false">E22+1</f>
+        <v>4</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1027,16 +1170,20 @@
       <c r="B23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C23" s="2" t="b">
+      <c r="C23" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1" t="n">
         <f aca="false">E22+0.1</f>
         <v>3.1</v>
       </c>
+      <c r="F23" s="2" t="n">
+        <f aca="false">E23+1</f>
+        <v>4.1</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -1045,16 +1192,20 @@
       <c r="B24" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C24" s="2" t="b">
+      <c r="C24" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E24" s="1" t="n">
         <f aca="false">E23+0.1</f>
         <v>3.2</v>
       </c>
+      <c r="F24" s="2" t="n">
+        <f aca="false">E24+1</f>
+        <v>4.2</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -1063,16 +1214,20 @@
       <c r="B25" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C25" s="2" t="b">
+      <c r="C25" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E25" s="1" t="n">
         <f aca="false">E24+0.1</f>
         <v>3.3</v>
       </c>
+      <c r="F25" s="2" t="n">
+        <f aca="false">E25+1</f>
+        <v>4.3</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -1081,16 +1236,20 @@
       <c r="B26" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C26" s="2" t="b">
+      <c r="C26" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E26" s="1" t="n">
         <f aca="false">E25+0.1</f>
         <v>3.4</v>
       </c>
+      <c r="F26" s="2" t="n">
+        <f aca="false">E26+1</f>
+        <v>4.4</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -1099,16 +1258,20 @@
       <c r="B27" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C27" s="2" t="b">
+      <c r="C27" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E27" s="1" t="n">
         <f aca="false">E26+0.1</f>
         <v>3.5</v>
       </c>
+      <c r="F27" s="2" t="n">
+        <f aca="false">E27+1</f>
+        <v>4.5</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -1117,16 +1280,20 @@
       <c r="B28" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C28" s="2" t="b">
+      <c r="C28" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E28" s="1" t="n">
         <f aca="false">E27+0.1</f>
         <v>3.6</v>
       </c>
+      <c r="F28" s="2" t="n">
+        <f aca="false">E28+1</f>
+        <v>4.6</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -1135,16 +1302,20 @@
       <c r="B29" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C29" s="2" t="b">
+      <c r="C29" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E29" s="1" t="n">
         <f aca="false">E28+0.1</f>
         <v>3.7</v>
       </c>
+      <c r="F29" s="2" t="n">
+        <f aca="false">E29+1</f>
+        <v>4.7</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
@@ -1153,16 +1324,20 @@
       <c r="B30" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C30" s="2" t="b">
+      <c r="C30" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E30" s="1" t="n">
         <f aca="false">E29+0.1</f>
         <v>3.8</v>
       </c>
+      <c r="F30" s="2" t="n">
+        <f aca="false">E30+1</f>
+        <v>4.8</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
@@ -1171,16 +1346,20 @@
       <c r="B31" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C31" s="2" t="b">
+      <c r="C31" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E31" s="1" t="n">
         <f aca="false">E30+0.1</f>
         <v>3.9</v>
       </c>
+      <c r="F31" s="2" t="n">
+        <f aca="false">E31+1</f>
+        <v>4.9</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
@@ -1189,16 +1368,20 @@
       <c r="B32" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C32" s="2" t="b">
+      <c r="C32" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E32" s="1" t="n">
         <f aca="false">E31+0.1</f>
         <v>4</v>
       </c>
+      <c r="F32" s="2" t="n">
+        <f aca="false">E32+1</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -1207,16 +1390,20 @@
       <c r="B33" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C33" s="2" t="b">
+      <c r="C33" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E33" s="1" t="n">
         <f aca="false">E32+0.1</f>
         <v>4.1</v>
       </c>
+      <c r="F33" s="2" t="n">
+        <f aca="false">E33+1</f>
+        <v>5.1</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
@@ -1225,16 +1412,20 @@
       <c r="B34" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C34" s="2" t="b">
+      <c r="C34" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E34" s="1" t="n">
         <f aca="false">E33+0.1</f>
         <v>4.2</v>
       </c>
+      <c r="F34" s="2" t="n">
+        <f aca="false">E34+1</f>
+        <v>5.2</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -1243,16 +1434,20 @@
       <c r="B35" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C35" s="2" t="b">
+      <c r="C35" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E35" s="1" t="n">
         <f aca="false">E34+0.1</f>
         <v>4.3</v>
       </c>
+      <c r="F35" s="2" t="n">
+        <f aca="false">E35+1</f>
+        <v>5.3</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
@@ -1261,16 +1456,20 @@
       <c r="B36" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C36" s="2" t="b">
+      <c r="C36" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E36" s="1" t="n">
         <f aca="false">E35+0.1</f>
         <v>4.4</v>
       </c>
+      <c r="F36" s="2" t="n">
+        <f aca="false">E36+1</f>
+        <v>5.4</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
@@ -1279,16 +1478,20 @@
       <c r="B37" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C37" s="2" t="b">
+      <c r="C37" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E37" s="1" t="n">
         <f aca="false">E36+0.1</f>
         <v>4.5</v>
       </c>
+      <c r="F37" s="2" t="n">
+        <f aca="false">E37+1</f>
+        <v>5.5</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
@@ -1297,16 +1500,20 @@
       <c r="B38" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C38" s="2" t="b">
+      <c r="C38" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E38" s="1" t="n">
         <f aca="false">E37+0.1</f>
         <v>4.6</v>
       </c>
+      <c r="F38" s="2" t="n">
+        <f aca="false">E38+1</f>
+        <v>5.6</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
@@ -1315,16 +1522,20 @@
       <c r="B39" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C39" s="2" t="b">
+      <c r="C39" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E39" s="1" t="n">
         <f aca="false">E38+0.1</f>
         <v>4.7</v>
       </c>
+      <c r="F39" s="2" t="n">
+        <f aca="false">E39+1</f>
+        <v>5.7</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
@@ -1333,16 +1544,20 @@
       <c r="B40" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C40" s="2" t="b">
+      <c r="C40" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">E39+0.1</f>
         <v>4.8</v>
       </c>
+      <c r="F40" s="2" t="n">
+        <f aca="false">E40+1</f>
+        <v>5.8</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
@@ -1351,16 +1566,20 @@
       <c r="B41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C41" s="2" t="b">
+      <c r="C41" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E41" s="1" t="n">
         <f aca="false">E40+0.1</f>
         <v>4.9</v>
       </c>
+      <c r="F41" s="2" t="n">
+        <f aca="false">E41+1</f>
+        <v>5.9</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -1369,16 +1588,20 @@
       <c r="B42" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C42" s="2" t="b">
+      <c r="C42" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E42" s="1" t="n">
         <f aca="false">E41+0.1</f>
         <v>5</v>
       </c>
+      <c r="F42" s="2" t="n">
+        <f aca="false">E42+1</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
@@ -1387,49 +1610,57 @@
       <c r="B43" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C43" s="2" t="b">
+      <c r="C43" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E43" s="1" t="n">
         <f aca="false">E42+0.1</f>
         <v>5.1</v>
       </c>
+      <c r="F43" s="2" t="n">
+        <f aca="false">E43+1</f>
+        <v>6.1</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E44" s="1" t="n">
         <v>100</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <f aca="false">E44+1</f>
+        <v>101</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="2"/>
+      <c r="C45" s="3"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="2"/>
+      <c r="C46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="2"/>
+      <c r="C47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="2"/>
+      <c r="C48" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>